<commit_message>
Don't let yourself be controlled by these three things: your past, people, and money.
</commit_message>
<xml_diff>
--- a/guo/bill.xlsx
+++ b/guo/bill.xlsx
@@ -24,10 +24,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17.6.18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>其他支出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -35,12 +31,16 @@
     <t>其他收入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>总计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +50,24 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -76,8 +94,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -382,34 +409,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="1">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1">
         <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>